<commit_message>
Uploading Agora/EI add-outputs, ccs, and ctrl-settings data files
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
+++ b/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
@@ -1,29 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\add-outputs\VoaSL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energyinnovation.sharepoint.com/sites/EUEPSModeling/Shared Documents/InputData_EI+Agora/add-outputs/VoaSL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E59E064-EF61-4312-82D8-C31F8060157D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E59E064-EF61-4312-82D8-C31F8060157D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="975" windowWidth="25830" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="VoaSL" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -45,43 +51,43 @@
     <t>Frequently Asked Questions on Mortality Risk Valuation</t>
   </si>
   <si>
+    <t>https://www.epa.gov/environmental-economics/mortality-risk-valuation#whatvalue</t>
+  </si>
+  <si>
+    <t>"What value of statistical life does EPA use?"</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>This variable is used to convert from dollars (in the SCoHIbP Social Cost of</t>
+  </si>
+  <si>
+    <t>Health Impacts by Pollutant variable) into human lives, so the VSL figure</t>
+  </si>
+  <si>
+    <t>here must reflect the one used to calculate the health impacts in that</t>
+  </si>
+  <si>
+    <t>variable for the result to be accurate.</t>
+  </si>
+  <si>
+    <t>Currency Year Adjustment</t>
+  </si>
+  <si>
     <t>We adjust 2006 dollars to 2012 dollars using the following conversion factor:</t>
   </si>
   <si>
     <t>See "cpi.xlsx" in the InputData folder for source information.</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>"What value of statistical life does EPA use?"</t>
+    <t>2012$/life</t>
   </si>
   <si>
     <t>Statistical Life</t>
   </si>
   <si>
-    <t>This variable is used to convert from dollars (in the SCoHIbP Social Cost of</t>
-  </si>
-  <si>
-    <t>Health Impacts by Pollutant variable) into human lives, so the VSL figure</t>
-  </si>
-  <si>
-    <t>here must reflect the one used to calculate the health impacts in that</t>
-  </si>
-  <si>
-    <t>variable for the result to be accurate.</t>
-  </si>
-  <si>
-    <t>Currency Year Adjustment</t>
-  </si>
-  <si>
-    <t>2012$/life</t>
-  </si>
-  <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>https://www.epa.gov/environmental-economics/mortality-risk-valuation#whatvalue</t>
   </si>
 </sst>
 </file>
@@ -134,7 +140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -144,7 +150,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -164,9 +169,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -204,9 +209,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,26 +244,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,26 +279,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -488,17 +459,17 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -506,72 +477,72 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>2013</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1.141</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -591,26 +562,26 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <f>7.4*10^6*About!A17</f>
@@ -620,4 +591,285 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
+    <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <xsd:import namespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="00484652-42e1-479e-92f4-fb0efddcdf60" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="eca5b831-c3dc-41cf-bd85-218b82cecb21" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c5b79d03-3bfd-4c46-9947-056a2403f6c9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91142F5A-8DE6-444F-A99F-323A9CD26AE0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B724F544-08C1-4D0E-9733-B1B41BD5E589}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21706FC7-BDC5-4584-923D-90B860A22E4E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Uploading newest US files
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
+++ b/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\add-outputs\VoaSL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Desktop\Dropbox_Free_Zone\EPS\Model Repos\eps-us\InputData\add-outputs\VoaSL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E59E064-EF61-4312-82D8-C31F8060157D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FF28FF-AE75-49F4-8013-0ABB667283AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="975" windowWidth="25830" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22200" yWindow="1920" windowWidth="21600" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="VoaSL" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>VoaSL Value of a Statistical Life</t>
   </si>
@@ -60,18 +60,6 @@
     <t>Statistical Life</t>
   </si>
   <si>
-    <t>This variable is used to convert from dollars (in the SCoHIbP Social Cost of</t>
-  </si>
-  <si>
-    <t>Health Impacts by Pollutant variable) into human lives, so the VSL figure</t>
-  </si>
-  <si>
-    <t>here must reflect the one used to calculate the health impacts in that</t>
-  </si>
-  <si>
-    <t>variable for the result to be accurate.</t>
-  </si>
-  <si>
     <t>Currency Year Adjustment</t>
   </si>
   <si>
@@ -82,6 +70,12 @@
   </si>
   <si>
     <t>https://www.epa.gov/environmental-economics/mortality-risk-valuation#whatvalue</t>
+  </si>
+  <si>
+    <t>This variable is used to convert estimated avoided premature mortalities</t>
+  </si>
+  <si>
+    <t>(calculated using data from HOIpTP) into a dollar amount.</t>
   </si>
 </sst>
 </file>
@@ -134,7 +128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -144,7 +138,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -164,9 +157,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -204,9 +197,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,26 +232,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,26 +267,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -484,9 +443,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -518,7 +479,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,45 +493,32 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
+      <c r="A15">
+        <v>1.141</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1.141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -602,7 +550,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>8</v>
@@ -610,10 +558,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <f>7.4*10^6*About!A17</f>
+        <f>7.4*10^6*About!A15</f>
         <v>8443400</v>
       </c>
     </row>

</xml_diff>